<commit_message>
Created test cases for the asia and europe markets on marketwatch.com, updated data sheet and test steps to reflect new test cases.
</commit_message>
<xml_diff>
--- a/com.marketwatch/src/test/resources/test_data.xlsx
+++ b/com.marketwatch/src/test/resources/test_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.marketwatch\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E490FD-1103-4229-9A03-0C9E851FC856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3AAF62-DE91-4581-80EF-C82E2506AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="USMarket" sheetId="1" r:id="rId1"/>
+    <sheet name="EuropeMarket" sheetId="2" r:id="rId2"/>
+    <sheet name="AsiaMarket" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Assertions</t>
   </si>
@@ -56,6 +58,42 @@
   </si>
   <si>
     <t>Crude Oil WTI (NYM $/bbl) Front Month</t>
+  </si>
+  <si>
+    <t>FTSE 100 Index</t>
+  </si>
+  <si>
+    <t>DAX</t>
+  </si>
+  <si>
+    <t>CAC 40 Index</t>
+  </si>
+  <si>
+    <t>FTSE MIB Index</t>
+  </si>
+  <si>
+    <t>IBEX 35 Index</t>
+  </si>
+  <si>
+    <t>STOXX Europe 600 Index</t>
+  </si>
+  <si>
+    <t>The Asia Dow Index USD</t>
+  </si>
+  <si>
+    <t>NIKKEI 225 Index</t>
+  </si>
+  <si>
+    <t>Hang Seng Index</t>
+  </si>
+  <si>
+    <t>Shanghai Composite Index</t>
+  </si>
+  <si>
+    <t>S&amp;P BSE Sensex Index</t>
+  </si>
+  <si>
+    <t>FTSE Straits Times Index</t>
   </si>
 </sst>
 </file>
@@ -417,9 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -464,4 +500,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641687E4-DD92-495D-B79E-84D3197FD0E8}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B39C1C-9BB3-40D5-A3B2-012E20FAD986}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test cases to market watch.
</commit_message>
<xml_diff>
--- a/com.marketwatch/src/test/resources/test_data.xlsx
+++ b/com.marketwatch/src/test/resources/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.marketwatch\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3AAF62-DE91-4581-80EF-C82E2506AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251D9A71-8CC2-4C2F-967A-3A6C66C445C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="3" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="USMarket" sheetId="1" r:id="rId1"/>
     <sheet name="EuropeMarket" sheetId="2" r:id="rId2"/>
     <sheet name="AsiaMarket" sheetId="3" r:id="rId3"/>
+    <sheet name="FXMarket" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Assertions</t>
   </si>
@@ -94,6 +95,24 @@
   </si>
   <si>
     <t>FTSE Straits Times Index</t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>Japanese Yen</t>
+  </si>
+  <si>
+    <t>British Pound</t>
+  </si>
+  <si>
+    <t>Australian Dollar</t>
+  </si>
+  <si>
+    <t>U.S. Dollar Index (DXY)</t>
+  </si>
+  <si>
+    <t>WSJ Dollar Index</t>
   </si>
 </sst>
 </file>
@@ -560,9 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B39C1C-9BB3-40D5-A3B2-012E20FAD986}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -608,4 +625,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021A62F4-D47D-487D-889F-60B7E4C7FB70}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>